<commit_message>
adding output files as csv
</commit_message>
<xml_diff>
--- a/data/IRS_data_mapping.xlsx
+++ b/data/IRS_data_mapping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="2260" windowWidth="27360" windowHeight="15880" tabRatio="500"/>
+    <workbookView xWindow="420" yWindow="1660" windowWidth="27360" windowHeight="15880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="173">
   <si>
     <t>year</t>
   </si>
@@ -787,9 +787,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>taxable_interest_count</t>
   </si>
   <si>
@@ -931,9 +928,6 @@
     <t>X__1</t>
   </si>
   <si>
-    <t>X__3</t>
-  </si>
-  <si>
     <t>X__16</t>
   </si>
   <si>
@@ -949,9 +943,6 @@
     <t>X__65</t>
   </si>
   <si>
-    <t>X__79</t>
-  </si>
-  <si>
     <t>ordinary_dividends_count</t>
   </si>
   <si>
@@ -1076,13 +1067,64 @@
   </si>
   <si>
     <t>paid_prep_count</t>
+  </si>
+  <si>
+    <t>X__40</t>
+  </si>
+  <si>
+    <t>X__2</t>
+  </si>
+  <si>
+    <t>X__69</t>
+  </si>
+  <si>
+    <t>X__14</t>
+  </si>
+  <si>
+    <t>X__15</t>
+  </si>
+  <si>
+    <t>X__29</t>
+  </si>
+  <si>
+    <t>X__30</t>
+  </si>
+  <si>
+    <t>X__39</t>
+  </si>
+  <si>
+    <t>X__49</t>
+  </si>
+  <si>
+    <t>X__52</t>
+  </si>
+  <si>
+    <t>X__53</t>
+  </si>
+  <si>
+    <t>X__61</t>
+  </si>
+  <si>
+    <t>X__62</t>
+  </si>
+  <si>
+    <t>X__63</t>
+  </si>
+  <si>
+    <t>X__71</t>
+  </si>
+  <si>
+    <t>X__72</t>
+  </si>
+  <si>
+    <t>X__73</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1119,6 +1161,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1137,23 +1186,48 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1429,10 +1503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E53" sqref="E3:E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.33203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -1442,12 +1516,18 @@
     <col min="4" max="16384" width="29.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D1" s="1">
+        <v>2011</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1455,10 +1535,10 @@
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1466,10 +1546,13 @@
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1477,10 +1560,13 @@
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1488,10 +1574,13 @@
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1499,10 +1588,13 @@
         <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1510,10 +1602,13 @@
         <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1521,10 +1616,13 @@
         <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1532,100 +1630,127 @@
         <v>17</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>26</v>
@@ -1633,10 +1758,13 @@
       <c r="D18" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>27</v>
@@ -1644,10 +1772,13 @@
       <c r="D19" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>28</v>
@@ -1655,10 +1786,13 @@
       <c r="D20" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>29</v>
@@ -1666,10 +1800,13 @@
       <c r="D21" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>30</v>
@@ -1677,10 +1814,13 @@
       <c r="D22" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>31</v>
@@ -1688,10 +1828,13 @@
       <c r="D23" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>32</v>
@@ -1699,10 +1842,13 @@
       <c r="D24" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>33</v>
@@ -1710,10 +1856,13 @@
       <c r="D25" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>34</v>
@@ -1721,120 +1870,153 @@
       <c r="D26" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>43</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>45</v>
@@ -1842,10 +2024,13 @@
       <c r="D37" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>46</v>
@@ -1853,32 +2038,41 @@
       <c r="D38" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>49</v>
@@ -1886,10 +2080,13 @@
       <c r="D41" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E41" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>50</v>
@@ -1897,32 +2094,41 @@
       <c r="D42" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E42" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>53</v>
@@ -1930,10 +2136,13 @@
       <c r="D45" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E45" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>54</v>
@@ -1941,32 +2150,41 @@
       <c r="D46" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E46" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>55</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>56</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>57</v>
@@ -1974,10 +2192,13 @@
       <c r="D49" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E49" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>58</v>
@@ -1985,53 +2206,60 @@
       <c r="D50" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E50" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>59</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D55" s="1">
+      <c r="D54" s="1">
         <v>2011</v>
       </c>
     </row>

</xml_diff>